<commit_message>
Add functionality to delete plants from database by removing their bed number and test said functionality
</commit_message>
<xml_diff>
--- a/server/src/main/resources/TestUpdateAccessionList2016.xlsx
+++ b/server/src/main/resources/TestUpdateAccessionList2016.xlsx
@@ -14,6 +14,7 @@
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'2016 Accession List Steves '!$A$4:$H$362</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'2016 Accession List Steves '!$A$4:$H$362</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'2016 Accession List Steves '!$A$4:$H$362</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'2016 Accession List Steves '!$A$4:$H$362</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1929" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1928" uniqueCount="568">
   <si>
     <t xml:space="preserve">2016 Accession List: Steve's Design</t>
   </si>
@@ -3556,24 +3557,24 @@
   <dimension ref="A1:Z454"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="G83" activeCellId="0" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.13917525773196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.639175257732"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.2319587628866"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3659793814433"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.63917525773196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0463917525773"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.9123711340206"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.3659793814433"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.7835051546392"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="73.6494845360825"/>
     <col collapsed="false" hidden="false" max="18" min="9" style="0" width="9.13917525773196"/>
-    <col collapsed="false" hidden="false" max="26" min="19" style="0" width="7.77319587628866"/>
-    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.59278350515464"/>
+    <col collapsed="false" hidden="false" max="26" min="19" style="0" width="7.63917525773196"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="8.45360824742268"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6935,9 +6936,6 @@
         <v>16</v>
       </c>
       <c r="F83" s="36"/>
-      <c r="G83" s="37" t="s">
-        <v>118</v>
-      </c>
       <c r="H83" s="38"/>
       <c r="I83" s="5"/>
       <c r="J83" s="5"/>

</xml_diff>